<commit_message>
finished runs of all scenarios, tentative
</commit_message>
<xml_diff>
--- a/carbon-tax-2000-simulation.xlsx
+++ b/carbon-tax-2000-simulation.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>10315.421612493</v>
+        <v>10315.42169401073</v>
       </c>
       <c r="C2" t="n">
-        <v>1137.022132255279</v>
+        <v>1137.022126809901</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2009.127989155639</v>
+        <v>2015.412030040912</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>9947.66041512731</v>
+        <v>9947.660470439747</v>
       </c>
       <c r="C3" t="n">
-        <v>1061.339585056932</v>
+        <v>1061.339581731656</v>
       </c>
       <c r="D3" t="n">
-        <v>5.820506735913863e-07</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>44.40294350132098</v>
+        <v>44.40310547356616</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>9734.038346669075</v>
+        <v>9734.038271254843</v>
       </c>
       <c r="C4" t="n">
-        <v>1091.961718252975</v>
+        <v>1091.961727104107</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2.809527484062984e-06</v>
       </c>
       <c r="E4" t="n">
-        <v>44.22186638514581</v>
+        <v>44.22186911782016</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>9971.392360120588</v>
+        <v>9971.392348114701</v>
       </c>
       <c r="C5" t="n">
-        <v>846.6076508289226</v>
+        <v>846.6076576251747</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>3.792324853504384e-06</v>
       </c>
       <c r="E5" t="n">
-        <v>44.31436515294163</v>
+        <v>44.3143613912041</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>9724.806910405483</v>
+        <v>9724.807265481928</v>
       </c>
       <c r="C6" t="n">
-        <v>1393.193092212358</v>
+        <v>1393.193070892443</v>
       </c>
       <c r="D6" t="n">
-        <v>5.109493986908101e-06</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>40.48786351003436</v>
+        <v>40.48794600661611</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>11155.89081587371</v>
+        <v>11155.89033387972</v>
       </c>
       <c r="C7" t="n">
-        <v>1086.10959720224</v>
+        <v>1086.109644575713</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>2.928675915208345e-05</v>
       </c>
       <c r="E7" t="n">
-        <v>53.24205438357458</v>
+        <v>53.24194507994822</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>13156.91827280813</v>
+        <v>13156.91817924211</v>
       </c>
       <c r="C8" t="n">
-        <v>1131.081693957522</v>
+        <v>1131.08174075436</v>
       </c>
       <c r="D8" t="n">
-        <v>3.320305950011413e-05</v>
+        <v>7.991684063266002e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>69.96971075580267</v>
+        <v>69.96964709000277</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +579,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>14369.80929696398</v>
+        <v>14369.80924388467</v>
       </c>
       <c r="C9" t="n">
-        <v>1423.190675267307</v>
+        <v>1423.190680712407</v>
       </c>
       <c r="D9" t="n">
-        <v>5.311247288329461e-05</v>
+        <v>7.53137063268494e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>71.11292901703182</v>
+        <v>71.11284599660347</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +596,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>15340.76620911916</v>
+        <v>15340.76559540257</v>
       </c>
       <c r="C10" t="n">
-        <v>956.2318905736793</v>
+        <v>956.2321903835378</v>
       </c>
       <c r="D10" t="n">
-        <v>0.001898412920001468</v>
+        <v>0.002211981849071495</v>
       </c>
       <c r="E10" t="n">
-        <v>101.9403010966147</v>
+        <v>101.9387118102505</v>
       </c>
     </row>
     <row r="11">
@@ -613,16 +613,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>15797.18354863849</v>
+        <v>15797.18218192384</v>
       </c>
       <c r="C11" t="n">
-        <v>688.4652948553539</v>
+        <v>688.4653749833706</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>302.7181392641137</v>
+        <v>300.5545218135926</v>
       </c>
     </row>
     <row r="12">
@@ -630,16 +630,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>15601.23101182825</v>
+        <v>15601.2526230667</v>
       </c>
       <c r="C12" t="n">
-        <v>1004.842995150667</v>
+        <v>1004.841087124326</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>920.9453431705273</v>
+        <v>923.8733193896476</v>
       </c>
     </row>
     <row r="13">
@@ -647,16 +647,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>15712.57432905749</v>
+        <v>15712.57216801122</v>
       </c>
       <c r="C13" t="n">
-        <v>907.4092648131686</v>
+        <v>907.4103439443916</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01638973759312408</v>
+        <v>0.01747058803239995</v>
       </c>
       <c r="E13" t="n">
-        <v>103.3647648100601</v>
+        <v>103.3737146004381</v>
       </c>
     </row>
     <row r="14">
@@ -664,16 +664,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>15500.3274371691</v>
+        <v>15500.32497151223</v>
       </c>
       <c r="C14" t="n">
-        <v>1013.860145294669</v>
+        <v>1013.860674491943</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>102.3357427702969</v>
+        <v>102.3507504197461</v>
       </c>
     </row>
     <row r="15">
@@ -681,16 +681,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>15354.37185383195</v>
+        <v>15354.34513742684</v>
       </c>
       <c r="C15" t="n">
-        <v>1131.678939573624</v>
+        <v>1131.681734355002</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>101.8856163709743</v>
+        <v>101.9048243945968</v>
       </c>
     </row>
     <row r="16">
@@ -698,16 +698,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>15371.35667135266</v>
+        <v>15371.34980884248</v>
       </c>
       <c r="C16" t="n">
-        <v>1053.647804022298</v>
+        <v>1053.649250906375</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>0.0009393024244496858</v>
       </c>
       <c r="E16" t="n">
-        <v>101.9054681511083</v>
+        <v>101.9061075166688</v>
       </c>
     </row>
     <row r="17">
@@ -715,16 +715,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>15128.14652602411</v>
+        <v>15128.14675858265</v>
       </c>
       <c r="C17" t="n">
-        <v>1349.85379721877</v>
+        <v>1349.853805114885</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>82.3411311725593</v>
+        <v>82.34124317866838</v>
       </c>
     </row>
     <row r="18">
@@ -732,16 +732,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>15270.67632409168</v>
+        <v>15270.67636275309</v>
       </c>
       <c r="C18" t="n">
-        <v>1564.323687079537</v>
+        <v>1564.323701143154</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>101.4417372962306</v>
+        <v>101.441726279094</v>
       </c>
     </row>
     <row r="19">
@@ -749,16 +749,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>15766.6831847527</v>
+        <v>15766.68303193526</v>
       </c>
       <c r="C19" t="n">
-        <v>1519.572912520418</v>
+        <v>1519.572917716377</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>696.7632266163009</v>
+        <v>703.3254997114586</v>
       </c>
     </row>
     <row r="20">
@@ -766,16 +766,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>16006.5410132529</v>
+        <v>16005.92946816655</v>
       </c>
       <c r="C20" t="n">
-        <v>1758.959778838409</v>
+        <v>1759.070745509823</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>253.1185611402739</v>
+        <v>106.6507327939511</v>
       </c>
     </row>
     <row r="21">
@@ -783,16 +783,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>15889.57307063896</v>
+        <v>15889.57344720714</v>
       </c>
       <c r="C21" t="n">
-        <v>1694.426939092899</v>
+        <v>1694.426889777404</v>
       </c>
       <c r="D21" t="n">
-        <v>1.463502773228141e-06</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>104.0901915134867</v>
+        <v>104.0897697816072</v>
       </c>
     </row>
     <row r="22">
@@ -800,16 +800,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>16388.35185937639</v>
+        <v>16388.35181969894</v>
       </c>
       <c r="C22" t="n">
-        <v>446.1905796141245</v>
+        <v>446.190583331682</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>493.0626697104354</v>
+        <v>482.9804668288408</v>
       </c>
     </row>
     <row r="23">
@@ -817,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>14963.04177076585</v>
+        <v>14963.04172808934</v>
       </c>
       <c r="C23" t="n">
-        <v>653.9582129423931</v>
+        <v>653.9582330745418</v>
       </c>
       <c r="D23" t="n">
-        <v>1.627554509832268e-05</v>
+        <v>3.879718720510096e-05</v>
       </c>
       <c r="E23" t="n">
-        <v>81.27120795024375</v>
+        <v>81.27147774024067</v>
       </c>
     </row>
     <row r="24">
@@ -834,16 +834,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>13154.66273687601</v>
+        <v>13154.66273927436</v>
       </c>
       <c r="C24" t="n">
-        <v>861.3372627244376</v>
+        <v>861.3372622070139</v>
       </c>
       <c r="D24" t="n">
-        <v>5.439977755289958e-07</v>
+        <v>1.184450790296827e-06</v>
       </c>
       <c r="E24" t="n">
-        <v>70.70193250102736</v>
+        <v>70.70194782448253</v>
       </c>
     </row>
     <row r="25">
@@ -851,16 +851,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>11515.70052443409</v>
+        <v>11515.70051045285</v>
       </c>
       <c r="C25" t="n">
-        <v>1086.299496745592</v>
+        <v>1086.299498546334</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>3.139291087599519e-07</v>
       </c>
       <c r="E25" t="n">
-        <v>62.1533884896111</v>
+        <v>62.15338867861517</v>
       </c>
     </row>
     <row r="26">
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>10516.23041874186</v>
+        <v>10516.2304187236</v>
       </c>
       <c r="C26" t="n">
-        <v>1167.776084501369</v>
+        <v>1167.776084501061</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>44.44970806769726</v>
+        <v>44.44970804089186</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>10291.22189735863</v>
+        <v>10291.22189736669</v>
       </c>
       <c r="C27" t="n">
-        <v>922.7733461967443</v>
+        <v>922.7733461928027</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0047516957093903</v>
+        <v>0.004751691604984546</v>
       </c>
       <c r="E27" t="n">
-        <v>44.49417171557783</v>
+        <v>44.49417176742504</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>9890.580773465252</v>
+        <v>9890.580773366093</v>
       </c>
       <c r="C28" t="n">
-        <v>1109.461057829308</v>
+        <v>1109.461057834514</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>44.31052394622893</v>
+        <v>44.31052391722046</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>9968.413024967704</v>
+        <v>9968.413024958549</v>
       </c>
       <c r="C29" t="n">
-        <v>972.5838517197658</v>
+        <v>972.5838517227189</v>
       </c>
       <c r="D29" t="n">
-        <v>0.003120186823635952</v>
+        <v>0.00312019304869502</v>
       </c>
       <c r="E29" t="n">
-        <v>44.33562413210618</v>
+        <v>44.33562415961295</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>10400.3971415409</v>
+        <v>10400.39714153165</v>
       </c>
       <c r="C30" t="n">
-        <v>838.59838623409</v>
+        <v>838.5983862384172</v>
       </c>
       <c r="D30" t="n">
-        <v>0.004467753215297124</v>
+        <v>0.004467758124205896</v>
       </c>
       <c r="E30" t="n">
-        <v>44.41509951202119</v>
+        <v>44.41509954953889</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>11187.43665705026</v>
+        <v>11187.43665702104</v>
       </c>
       <c r="C31" t="n">
-        <v>1149.56132814381</v>
+        <v>1149.561328158457</v>
       </c>
       <c r="D31" t="n">
-        <v>0.002012794236978377</v>
+        <v>0.002012808779424264</v>
       </c>
       <c r="E31" t="n">
-        <v>49.5207905490897</v>
+        <v>49.52079056997493</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>13317.02039766053</v>
+        <v>13317.02039767132</v>
       </c>
       <c r="C32" t="n">
-        <v>1025.588773022326</v>
+        <v>1025.588773021695</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>811.9729184458755</v>
+        <v>811.9729188213282</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>15134.11561263217</v>
+        <v>15134.11561263194</v>
       </c>
       <c r="C33" t="n">
-        <v>779.8840375947022</v>
+        <v>779.8840375947767</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0003494238452291181</v>
+        <v>0.0003494239490256401</v>
       </c>
       <c r="E33" t="n">
-        <v>101.7418409324264</v>
+        <v>101.7418409311848</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>15613.93716484261</v>
+        <v>15613.93716484404</v>
       </c>
       <c r="C34" t="n">
-        <v>799.31851329311</v>
+        <v>799.3185132930511</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>653.0889335779955</v>
+        <v>653.0889341932784</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>15936.11517763487</v>
+        <v>15936.11517763855</v>
       </c>
       <c r="C35" t="n">
-        <v>649.1356378330916</v>
+        <v>649.1356378326091</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>106.3468814967156</v>
+        <v>106.3468815071808</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>16200.61152217852</v>
+        <v>16200.61152217937</v>
       </c>
       <c r="C36" t="n">
-        <v>490.3928595461533</v>
+        <v>490.392859546025</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>302.0792128308073</v>
+        <v>302.0792128291468</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>16164.30265546353</v>
+        <v>16164.30265546345</v>
       </c>
       <c r="C37" t="n">
-        <v>487.1359222550615</v>
+        <v>487.1359222548982</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>361.3012823389647</v>
+        <v>361.301283528083</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>15904.30743140078</v>
+        <v>15904.30743139676</v>
       </c>
       <c r="C38" t="n">
-        <v>574.7278134368701</v>
+        <v>574.727813437152</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>106.2029511919861</v>
+        <v>106.202951193822</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>15635.84931840373</v>
+        <v>15635.84931840403</v>
       </c>
       <c r="C39" t="n">
-        <v>731.1506753000956</v>
+        <v>731.150675300133</v>
       </c>
       <c r="D39" t="n">
-        <v>6.289854590352511e-06</v>
+        <v>6.289500908522038e-06</v>
       </c>
       <c r="E39" t="n">
-        <v>102.9981021742018</v>
+        <v>102.9981021731682</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>15337.6872631885</v>
+        <v>15337.68726318714</v>
       </c>
       <c r="C40" t="n">
-        <v>835.3142246852726</v>
+        <v>835.3142246853599</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>101.7881852269672</v>
+        <v>101.7881852260834</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>15195.17738001615</v>
+        <v>15195.17738001683</v>
       </c>
       <c r="C41" t="n">
-        <v>898.8216118464039</v>
+        <v>898.8216118462828</v>
       </c>
       <c r="D41" t="n">
-        <v>0.001007130457945881</v>
+        <v>0.001007129929549728</v>
       </c>
       <c r="E41" t="n">
-        <v>82.48706083961829</v>
+        <v>82.48706084080374</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>15306.27508044933</v>
+        <v>15306.27508045257</v>
       </c>
       <c r="C42" t="n">
-        <v>918.7303494106881</v>
+        <v>918.7303494100395</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>101.6844600714306</v>
+        <v>101.6844600697032</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>15498.34698846726</v>
+        <v>15498.34698846614</v>
       </c>
       <c r="C43" t="n">
-        <v>1014.651827916031</v>
+        <v>1014.651827916748</v>
       </c>
       <c r="D43" t="n">
-        <v>0.001182434373787339</v>
+        <v>0.001182434790282866</v>
       </c>
       <c r="E43" t="n">
-        <v>102.3260522869083</v>
+        <v>102.3260522919479</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>15951.34855102137</v>
+        <v>15951.34855102191</v>
       </c>
       <c r="C44" t="n">
-        <v>1050.719965302571</v>
+        <v>1050.719965302628</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>780.1352947726153</v>
+        <v>780.135294928486</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>15733.99961728038</v>
+        <v>15733.99961728089</v>
       </c>
       <c r="C45" t="n">
-        <v>989.9959487394932</v>
+        <v>989.9959487394784</v>
       </c>
       <c r="D45" t="n">
-        <v>0.004429550943790231</v>
+        <v>0.004429550491522065</v>
       </c>
       <c r="E45" t="n">
-        <v>103.5423559621031</v>
+        <v>103.5423559597862</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>15271.78624513612</v>
+        <v>15271.78624513565</v>
       </c>
       <c r="C46" t="n">
-        <v>809.2245285760423</v>
+        <v>809.2245285758038</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>102.1105830466089</v>
+        <v>102.110583046141</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>14331.28058775256</v>
+        <v>14331.2805877519</v>
       </c>
       <c r="C47" t="n">
-        <v>845.7199123800399</v>
+        <v>845.7199123799246</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>71.78223406856696</v>
+        <v>71.78223406827587</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>13102.02948853338</v>
+        <v>13102.02948853357</v>
       </c>
       <c r="C48" t="n">
-        <v>770.9702351019504</v>
+        <v>770.9702351019505</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0002760886242364641</v>
+        <v>0.000276088395908672</v>
       </c>
       <c r="E48" t="n">
-        <v>70.39608610338516</v>
+        <v>70.39608610485995</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>11822.44298054601</v>
+        <v>11822.44298054485</v>
       </c>
       <c r="C49" t="n">
-        <v>777.5570598969628</v>
+        <v>777.5570598968757</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>63.47782543263784</v>
+        <v>63.47782543249131</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>10851.05607599447</v>
+        <v>10851.05614759156</v>
       </c>
       <c r="C50" t="n">
-        <v>837.9439240027391</v>
+        <v>837.9439196346666</v>
       </c>
       <c r="D50" t="n">
-        <v>2.804109407193565e-09</v>
+        <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>46.1234413242147</v>
+        <v>46.12341483479319</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>10318.49323422741</v>
+        <v>10318.49318686367</v>
       </c>
       <c r="C51" t="n">
-        <v>832.5067659860221</v>
+        <v>832.5067896350608</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>2.347780720928941e-05</v>
       </c>
       <c r="E51" t="n">
-        <v>44.4050086471378</v>
+        <v>44.40495365524533</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1310,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>10335.21492800334</v>
+        <v>10335.21492102454</v>
       </c>
       <c r="C52" t="n">
-        <v>518.7850719997895</v>
+        <v>518.7850754980873</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>3.473891143896447e-06</v>
       </c>
       <c r="E52" t="n">
-        <v>44.47209436162246</v>
+        <v>44.47217208196479</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>10324.96619999971</v>
+        <v>10324.9663920293</v>
       </c>
       <c r="C53" t="n">
-        <v>403.0338000001831</v>
+        <v>403.0337880887472</v>
       </c>
       <c r="D53" t="n">
-        <v>3.66582583284401e-10</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>44.46964746296923</v>
+        <v>44.46955589675269</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1344,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>10335.30635395178</v>
+        <v>10335.30634178409</v>
       </c>
       <c r="C54" t="n">
-        <v>469.6936460239756</v>
+        <v>469.693652127862</v>
       </c>
       <c r="D54" t="n">
-        <v>2.421175700251185e-08</v>
+        <v>6.081954188179715e-06</v>
       </c>
       <c r="E54" t="n">
-        <v>44.47211610956617</v>
+        <v>44.47201540233695</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1361,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>10568.10077678979</v>
+        <v>10568.10076249838</v>
       </c>
       <c r="C55" t="n">
-        <v>581.8992239509279</v>
+        <v>581.8992307622955</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>6.73259482368261e-06</v>
       </c>
       <c r="E55" t="n">
-        <v>44.47836044810534</v>
+        <v>44.47856836761158</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1378,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>11334.26514036839</v>
+        <v>11334.26520175539</v>
       </c>
       <c r="C56" t="n">
-        <v>524.7348600684834</v>
+        <v>524.7348560679239</v>
       </c>
       <c r="D56" t="n">
-        <v>6.80222016806052e-08</v>
+        <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>50.61249556616279</v>
+        <v>50.61254478525905</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1395,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>12610.37299032596</v>
+        <v>12610.37287978718</v>
       </c>
       <c r="C57" t="n">
-        <v>458.6271014731122</v>
+        <v>458.6271141383331</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>6.068447919132673e-06</v>
       </c>
       <c r="E57" t="n">
-        <v>69.40162410050291</v>
+        <v>69.40159205339397</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1412,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>13700.01468495986</v>
+        <v>13699.76270547739</v>
       </c>
       <c r="C58" t="n">
-        <v>538.2054483781189</v>
+        <v>538.2372945847279</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>5.897043586412184e-07</v>
       </c>
       <c r="E58" t="n">
-        <v>1118.684591139974</v>
+        <v>70.34289517358546</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>14525.18784219158</v>
+        <v>14525.18402367301</v>
       </c>
       <c r="C59" t="n">
-        <v>476.8157876421613</v>
+        <v>476.8161556205607</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>74.10882478593331</v>
+        <v>72.46496860563593</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1446,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>14775.30327024481</v>
+        <v>14774.90287368669</v>
       </c>
       <c r="C60" t="n">
-        <v>461.0593960700404</v>
+        <v>461.0965204977916</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>0.0006052100990631808</v>
       </c>
       <c r="E60" t="n">
-        <v>101.9345553976991</v>
+        <v>102.0101458876252</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1463,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>14776.10133627076</v>
+        <v>14776.39008754727</v>
       </c>
       <c r="C61" t="n">
-        <v>436.8732877594825</v>
+        <v>436.8260640342598</v>
       </c>
       <c r="D61" t="n">
-        <v>0.02535062062565563</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>101.9976437609223</v>
+        <v>102.0216435062448</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1480,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>14595.34535194114</v>
+        <v>14595.26833870484</v>
       </c>
       <c r="C62" t="n">
-        <v>354.6545743216291</v>
+        <v>354.6931253072826</v>
       </c>
       <c r="D62" t="n">
-        <v>8.2263424977979e-05</v>
+        <v>0.03849749275341462</v>
       </c>
       <c r="E62" t="n">
-        <v>72.27614158345588</v>
+        <v>101.6625804429708</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1497,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>14383.32785343482</v>
+        <v>14383.32735062683</v>
       </c>
       <c r="C63" t="n">
-        <v>242.6721680460079</v>
+        <v>242.6724099728298</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>0.0002391611888663356</v>
       </c>
       <c r="E63" t="n">
-        <v>71.90279169495226</v>
+        <v>71.90238668888696</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>14156.65900230311</v>
+        <v>14156.65927230842</v>
       </c>
       <c r="C64" t="n">
-        <v>194.341003498667</v>
+        <v>194.3409818337511</v>
       </c>
       <c r="D64" t="n">
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>71.09590955302859</v>
+        <v>71.09594468209696</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1531,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>14066.20268203207</v>
+        <v>14066.2026794649</v>
       </c>
       <c r="C65" t="n">
-        <v>167.7973179962679</v>
+        <v>167.7973192695015</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>1.264350754134242e-06</v>
       </c>
       <c r="E65" t="n">
-        <v>70.83860920809053</v>
+        <v>70.8386074726324</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1548,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>14264.13529583486</v>
+        <v>14264.13529786277</v>
       </c>
       <c r="C66" t="n">
-        <v>217.8647040824559</v>
+        <v>217.8647038487231</v>
       </c>
       <c r="D66" t="n">
-        <v>8.260136421522065e-08</v>
+        <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>71.46107956603986</v>
+        <v>71.46107838303705</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1565,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>14585.75169355941</v>
+        <v>14585.75173016145</v>
       </c>
       <c r="C67" t="n">
-        <v>398.2483041071666</v>
+        <v>398.2482966954275</v>
       </c>
       <c r="D67" t="n">
-        <v>2.331086056255055e-06</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>101.7128192657218</v>
+        <v>101.712776984011</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1582,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>14761.3429475795</v>
+        <v>14761.34289129727</v>
       </c>
       <c r="C68" t="n">
-        <v>870.2445516796572</v>
+        <v>870.2445542349489</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>638.572894192888</v>
+        <v>645.4734469913434</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1599,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>14299.27166024493</v>
+        <v>14299.27165992235</v>
       </c>
       <c r="C69" t="n">
-        <v>1194.728339980037</v>
+        <v>1194.72834003884</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>3.8795562054658e-08</v>
       </c>
       <c r="E69" t="n">
-        <v>71.580454957847</v>
+        <v>71.58045526224375</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1616,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>13608.1058255797</v>
+        <v>13608.10583552261</v>
       </c>
       <c r="C70" t="n">
-        <v>1360.894174210488</v>
+        <v>1360.894173312954</v>
       </c>
       <c r="D70" t="n">
-        <v>2.095905793950201e-07</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>70.8308385661192</v>
+        <v>70.81182076922826</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1633,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>12729.5023135082</v>
+        <v>12729.5022970963</v>
       </c>
       <c r="C71" t="n">
-        <v>1468.497697240568</v>
+        <v>1468.497700456008</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>2.445260122820979e-06</v>
       </c>
       <c r="E71" t="n">
-        <v>70.81546297571731</v>
+        <v>69.94529797213833</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1650,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>11667.11927950319</v>
+        <v>11667.11964552879</v>
       </c>
       <c r="C72" t="n">
-        <v>1511.880714258984</v>
+        <v>1511.880685602513</v>
       </c>
       <c r="D72" t="n">
-        <v>6.231617143262554e-06</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>63.0376612317982</v>
+        <v>63.03772972639366</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1667,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>10942.50089591207</v>
+        <v>10942.50090020027</v>
       </c>
       <c r="C73" t="n">
-        <v>1176.499104044183</v>
+        <v>1176.499103806358</v>
       </c>
       <c r="D73" t="n">
-        <v>4.372416864020474e-08</v>
+        <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>48.91953271280143</v>
+        <v>48.91953447740166</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1684,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>10347.55668292391</v>
+        <v>10347.5555482299</v>
       </c>
       <c r="C74" t="n">
-        <v>849.4433076021985</v>
+        <v>849.4438869518451</v>
       </c>
       <c r="D74" t="n">
-        <v>9.464465791919876e-06</v>
+        <v>0.0005642546689369935</v>
       </c>
       <c r="E74" t="n">
-        <v>46.89957081404846</v>
+        <v>46.90346294454601</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1701,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>9560.455374320445</v>
+        <v>9560.45217214416</v>
       </c>
       <c r="C75" t="n">
-        <v>708.5466255748556</v>
+        <v>708.5473288464284</v>
       </c>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>0.000498512851892682</v>
       </c>
       <c r="E75" t="n">
-        <v>41.62101553965331</v>
+        <v>41.63756833315225</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>10057.8578619193</v>
+        <v>10057.85604861746</v>
       </c>
       <c r="C76" t="n">
-        <v>553.1417327810809</v>
+        <v>553.1426694305695</v>
       </c>
       <c r="D76" t="n">
-        <v>0.0004048947803353272</v>
+        <v>0.001280672868248641</v>
       </c>
       <c r="E76" t="n">
-        <v>44.49930149546455</v>
+        <v>44.4530538564843</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1735,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>9909.284484039632</v>
+        <v>9909.271214385028</v>
       </c>
       <c r="C77" t="n">
-        <v>416.7200339035477</v>
+        <v>416.7245989451989</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>0.0041824899604339</v>
       </c>
       <c r="E77" t="n">
-        <v>44.40633998178063</v>
+        <v>44.39342063372665</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>9804.274159311415</v>
+        <v>9804.361105091275</v>
       </c>
       <c r="C78" t="n">
-        <v>457.7254198292906</v>
+        <v>457.7202277941904</v>
       </c>
       <c r="D78" t="n">
-        <v>0.0004204389135631817</v>
+        <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>44.39215182596876</v>
+        <v>44.37448841163587</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>9857.854093612485</v>
+        <v>9857.850080515742</v>
       </c>
       <c r="C79" t="n">
-        <v>523.1451424156988</v>
+        <v>523.1471909274345</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0007632087180147779</v>
+        <v>0.002725831967351485</v>
       </c>
       <c r="E79" t="n">
-        <v>44.32067786257098</v>
+        <v>44.35370232858239</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +1786,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>10125.9284952358</v>
+        <v>10125.89771078168</v>
       </c>
       <c r="C80" t="n">
-        <v>551.1093477459326</v>
+        <v>551.1111156552147</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>44.65157812495412</v>
+        <v>44.50898826274509</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>10661.84850700351</v>
+        <v>10660.52756663693</v>
       </c>
       <c r="C81" t="n">
-        <v>513.3416275958277</v>
+        <v>513.4762138043363</v>
       </c>
       <c r="D81" t="n">
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>345.7956456002361</v>
+        <v>45.2192885084171</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +1820,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>11527.89435119757</v>
+        <v>11526.93275226282</v>
       </c>
       <c r="C82" t="n">
-        <v>532.0086780879976</v>
+        <v>532.0706809356548</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>62.53722051461334</v>
+        <v>62.40756231167623</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +1837,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>12621.58122456903</v>
+        <v>12621.42493925841</v>
       </c>
       <c r="C83" t="n">
-        <v>333.5921176919596</v>
+        <v>333.602874058938</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>69.54647074512842</v>
+        <v>69.50917544473396</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +1854,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>13290.23144252012</v>
+        <v>13289.73979659626</v>
       </c>
       <c r="C84" t="n">
-        <v>304.223312794188</v>
+        <v>304.2792743250886</v>
       </c>
       <c r="D84" t="n">
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>1738.771357060778</v>
+        <v>70.23978565899306</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +1871,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>13651.87423291476</v>
+        <v>13651.85470117479</v>
       </c>
       <c r="C85" t="n">
-        <v>310.1442348659248</v>
+        <v>310.1455224315046</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>70.49436018150185</v>
+        <v>70.40098461065216</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +1888,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>13753.27708414057</v>
+        <v>13753.28086681991</v>
       </c>
       <c r="C86" t="n">
-        <v>347.7200762159159</v>
+        <v>347.7181647223702</v>
       </c>
       <c r="D86" t="n">
-        <v>0.002836808014461349</v>
+        <v>0.0009674902939852455</v>
       </c>
       <c r="E86" t="n">
-        <v>70.47066304279893</v>
+        <v>70.48151619313049</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +1905,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>13628.98469718996</v>
+        <v>13628.98277260047</v>
       </c>
       <c r="C87" t="n">
-        <v>415.0280155035987</v>
+        <v>415.0280665136567</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>70.16918136785991</v>
+        <v>70.16389447610709</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +1922,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>13450.20618208446</v>
+        <v>13450.20568261252</v>
       </c>
       <c r="C88" t="n">
-        <v>446.7937105904113</v>
+        <v>446.7939633860899</v>
       </c>
       <c r="D88" t="n">
-        <v>0.0001072178521736473</v>
+        <v>0.0003536479795947338</v>
       </c>
       <c r="E88" t="n">
-        <v>69.83801919623794</v>
+        <v>69.8396576832709</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +1939,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>13515.91009185869</v>
+        <v>13515.91058976306</v>
       </c>
       <c r="C89" t="n">
-        <v>302.0914192205904</v>
+        <v>302.0913791538067</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>69.9559399839718</v>
+        <v>69.95629695962491</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +1956,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>13786.92084756384</v>
+        <v>13786.92223097932</v>
       </c>
       <c r="C90" t="n">
-        <v>257.0786847224197</v>
+        <v>257.0781991568874</v>
       </c>
       <c r="D90" t="n">
-        <v>0.0004672467139079433</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>70.56172954733893</v>
+        <v>70.56317716570091</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +1973,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>14003.55736667578</v>
+        <v>14003.55501380087</v>
       </c>
       <c r="C91" t="n">
-        <v>531.4442766737029</v>
+        <v>531.4447030740422</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>0.0002828424896510644</v>
       </c>
       <c r="E91" t="n">
-        <v>70.88763411426028</v>
+        <v>70.88684378741485</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +1990,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>14290.36938877817</v>
+        <v>14290.36553297038</v>
       </c>
       <c r="C92" t="n">
-        <v>706.6342296859279</v>
+        <v>706.634563650927</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>71.45379070949599</v>
+        <v>71.45536786153936</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2007,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>14814.88799435884</v>
+        <v>14814.79563438723</v>
       </c>
       <c r="C93" t="n">
-        <v>819.299762741475</v>
+        <v>819.3047954745859</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>1068.458713819318</v>
+        <v>933.9929129111028</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2024,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>14723.20521876993</v>
+        <v>14723.23025940421</v>
       </c>
       <c r="C94" t="n">
-        <v>834.7914307518661</v>
+        <v>834.7863962175811</v>
       </c>
       <c r="D94" t="n">
-        <v>0.003347131115350409</v>
+        <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>101.7017314699278</v>
+        <v>101.7081047005328</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2041,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>13952.2077820823</v>
+        <v>13952.20795824996</v>
       </c>
       <c r="C95" t="n">
-        <v>697.7921959888602</v>
+        <v>697.7921629122768</v>
       </c>
       <c r="D95" t="n">
-        <v>2.190696212279724e-05</v>
+        <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>71.30448142347744</v>
+        <v>71.30456486203306</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2058,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>12811.67932350619</v>
+        <v>12811.67868651348</v>
       </c>
       <c r="C96" t="n">
-        <v>658.3211977998507</v>
+        <v>658.3212747251183</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>3.87226894133938e-05</v>
       </c>
       <c r="E96" t="n">
-        <v>70.42509416946092</v>
+        <v>70.42465990728228</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2075,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>11553.40943307551</v>
+        <v>11553.41112073052</v>
       </c>
       <c r="C97" t="n">
-        <v>724.5905699071322</v>
+        <v>724.5904625192346</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>62.37360306490129</v>
+        <v>62.37378640435835</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2092,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>11014.18247543837</v>
+        <v>11014.182475791</v>
       </c>
       <c r="C98" t="n">
-        <v>669.8175069488891</v>
+        <v>669.8175067370709</v>
       </c>
       <c r="D98" t="n">
-        <v>1.759512840471525e-05</v>
+        <v>1.745440276721177e-05</v>
       </c>
       <c r="E98" t="n">
-        <v>49.04529606653402</v>
+        <v>49.04529602138363</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2109,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>10540.55451774707</v>
+        <v>10540.55452174499</v>
       </c>
       <c r="C99" t="n">
-        <v>673.4458210714688</v>
+        <v>673.4458208375092</v>
       </c>
       <c r="D99" t="n">
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>44.49860530758929</v>
+        <v>44.49860538631644</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2126,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>10476.72658513045</v>
+        <v>10476.72658125842</v>
       </c>
       <c r="C100" t="n">
-        <v>523.2746005181044</v>
+        <v>523.2746012538603</v>
       </c>
       <c r="D100" t="n">
         <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>44.49432584371696</v>
+        <v>44.49432624392914</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2143,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>10607.37826158682</v>
+        <v>10607.37826262124</v>
       </c>
       <c r="C101" t="n">
-        <v>333.6223204023335</v>
+        <v>333.6223203381534</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>44.51360317526424</v>
+        <v>44.51360328577135</v>
       </c>
     </row>
     <row r="102">
@@ -2160,16 +2160,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>10870.25204598418</v>
+        <v>10870.25204537006</v>
       </c>
       <c r="C102" t="n">
-        <v>368.7479919834</v>
+        <v>368.7479919817706</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>46.15436605605292</v>
+        <v>46.15436604813539</v>
       </c>
     </row>
     <row r="103">
@@ -2177,16 +2177,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>11902.23181421877</v>
+        <v>11902.23181437015</v>
       </c>
       <c r="C103" t="n">
-        <v>434.7693274264079</v>
+        <v>434.7693273652719</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>63.98034201650603</v>
+        <v>63.98034190551719</v>
       </c>
     </row>
     <row r="104">
@@ -2194,16 +2194,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>13884.60770835331</v>
+        <v>13884.60770937142</v>
       </c>
       <c r="C104" t="n">
-        <v>457.4632688610228</v>
+        <v>457.4632687457736</v>
       </c>
       <c r="D104" t="n">
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>1213.891860518058</v>
+        <v>1213.89175024282</v>
       </c>
     </row>
     <row r="105">
@@ -2211,16 +2211,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>15478.17307844344</v>
+        <v>15478.17306125124</v>
       </c>
       <c r="C105" t="n">
-        <v>435.7532997133662</v>
+        <v>435.7533083078484</v>
       </c>
       <c r="D105" t="n">
-        <v>0.07354831930239944</v>
+        <v>0.07355690833103543</v>
       </c>
       <c r="E105" t="n">
-        <v>103.0465288113435</v>
+        <v>103.0465334609019</v>
       </c>
     </row>
     <row r="106">
@@ -2228,16 +2228,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>16088.83501185758</v>
+        <v>16088.83501289817</v>
       </c>
       <c r="C106" t="n">
-        <v>324.6904048221922</v>
+        <v>324.690404769446</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>281.0083396905097</v>
+        <v>281.0085577812322</v>
       </c>
     </row>
     <row r="107">
@@ -2245,16 +2245,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>16320.37100772063</v>
+        <v>16320.37100770369</v>
       </c>
       <c r="C107" t="n">
-        <v>264.6290085076996</v>
+        <v>264.6290085163822</v>
       </c>
       <c r="D107" t="n">
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>186.7924288838136</v>
+        <v>186.7924288862072</v>
       </c>
     </row>
     <row r="108">
@@ -2262,16 +2262,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>16448.60476012735</v>
+        <v>16448.6047601341</v>
       </c>
       <c r="C108" t="n">
-        <v>242.3952388444715</v>
+        <v>242.3952388414121</v>
       </c>
       <c r="D108" t="n">
-        <v>1.027299240871048e-06</v>
+        <v>1.023518688071543e-06</v>
       </c>
       <c r="E108" t="n">
-        <v>302.1086822038234</v>
+        <v>302.1086822025898</v>
       </c>
     </row>
     <row r="109">
@@ -2279,16 +2279,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>16422.0837130295</v>
+        <v>16422.08371305533</v>
       </c>
       <c r="C109" t="n">
-        <v>229.3762563386316</v>
+        <v>229.3762563351747</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>319.2560820073106</v>
+        <v>319.2562907692147</v>
       </c>
     </row>
     <row r="110">
@@ -2296,16 +2296,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>16260.26972991745</v>
+        <v>16260.26972991729</v>
       </c>
       <c r="C110" t="n">
-        <v>218.7302700634262</v>
+        <v>218.7302700627125</v>
       </c>
       <c r="D110" t="n">
-        <v>1.911978019927032e-08</v>
+        <v>1.994431414688324e-08</v>
       </c>
       <c r="E110" t="n">
-        <v>185.0959666439382</v>
+        <v>185.0959666436951</v>
       </c>
     </row>
     <row r="111">
@@ -2313,16 +2313,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>16158.80873794689</v>
+        <v>16158.80873794295</v>
       </c>
       <c r="C111" t="n">
-        <v>208.5548844424603</v>
+        <v>208.5548844425167</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>403.6643781021273</v>
+        <v>403.6645327438829</v>
       </c>
     </row>
     <row r="112">
@@ -2330,16 +2330,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>15945.99017639323</v>
+        <v>15945.99017640446</v>
       </c>
       <c r="C112" t="n">
-        <v>227.009859544996</v>
+        <v>227.0098595450051</v>
       </c>
       <c r="D112" t="n">
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>106.2233337378874</v>
+        <v>106.223333739268</v>
       </c>
     </row>
     <row r="113">
@@ -2347,16 +2347,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>15873.40923390224</v>
+        <v>15873.4092337288</v>
       </c>
       <c r="C113" t="n">
-        <v>220.5911113862677</v>
+        <v>220.5911114062254</v>
       </c>
       <c r="D113" t="n">
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>103.9352829261556</v>
+        <v>103.9352826635803</v>
       </c>
     </row>
     <row r="114">
@@ -2364,16 +2364,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>15926.24269495187</v>
+        <v>15926.24269482315</v>
       </c>
       <c r="C114" t="n">
-        <v>298.9609630706946</v>
+        <v>298.9609630785067</v>
       </c>
       <c r="D114" t="n">
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>710.8991427774409</v>
+        <v>710.8992258162477</v>
       </c>
     </row>
     <row r="115">
@@ -2381,16 +2381,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>16012.00720751009</v>
+        <v>16012.00720750383</v>
       </c>
       <c r="C115" t="n">
-        <v>500.9927522741372</v>
+        <v>500.9927522772157</v>
       </c>
       <c r="D115" t="n">
-        <v>4.017562564266352e-05</v>
+        <v>4.01787234364439e-05</v>
       </c>
       <c r="E115" t="n">
-        <v>106.5594979669405</v>
+        <v>106.5594979780701</v>
       </c>
     </row>
     <row r="116">
@@ -2398,16 +2398,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>16561.5557876829</v>
+        <v>16561.55578768656</v>
       </c>
       <c r="C116" t="n">
-        <v>440.6040379972052</v>
+        <v>440.6040379973674</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>878.0859361777824</v>
+        <v>878.086015397314</v>
       </c>
     </row>
     <row r="117">
@@ -2415,16 +2415,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>16438.40032487601</v>
+        <v>16438.40032488287</v>
       </c>
       <c r="C117" t="n">
-        <v>285.5996758843651</v>
+        <v>285.5996758845629</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>301.9250058211366</v>
+        <v>301.9250058211642</v>
       </c>
     </row>
     <row r="118">
@@ -2432,16 +2432,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>15925.45285030806</v>
+        <v>15925.4528503118</v>
       </c>
       <c r="C118" t="n">
-        <v>155.8428693969896</v>
+        <v>155.8428693973017</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>660.4965596853496</v>
+        <v>660.4966779446061</v>
       </c>
     </row>
     <row r="119">
@@ -2449,16 +2449,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>15046.97095517182</v>
+        <v>15046.97095519243</v>
       </c>
       <c r="C119" t="n">
-        <v>130.0290961232792</v>
+        <v>130.0290961222182</v>
       </c>
       <c r="D119" t="n">
         <v>0</v>
       </c>
       <c r="E119" t="n">
-        <v>81.26346358909237</v>
+        <v>81.26346359953638</v>
       </c>
     </row>
     <row r="120">
@@ -2466,16 +2466,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>13780.92919256885</v>
+        <v>13780.92919256634</v>
       </c>
       <c r="C120" t="n">
-        <v>92.07080283901755</v>
+        <v>92.0708028402068</v>
       </c>
       <c r="D120" t="n">
-        <v>4.794853539315922e-06</v>
+        <v>4.79556384618359e-06</v>
       </c>
       <c r="E120" t="n">
-        <v>71.71548648534366</v>
+        <v>71.71548647514808</v>
       </c>
     </row>
     <row r="121">
@@ -2483,16 +2483,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>12507.53866701729</v>
+        <v>12507.53866703955</v>
       </c>
       <c r="C121" t="n">
-        <v>92.46137485118111</v>
+        <v>92.46137485041996</v>
       </c>
       <c r="D121" t="n">
         <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>70.02965789725434</v>
+        <v>70.02965790310982</v>
       </c>
     </row>
     <row r="122">
@@ -2500,16 +2500,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>11598.22653967723</v>
+        <v>11598.22653967666</v>
       </c>
       <c r="C122" t="n">
-        <v>90.79461950165032</v>
+        <v>90.79461950168351</v>
       </c>
       <c r="D122" t="n">
         <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>64.43527266860362</v>
+        <v>64.43527267119501</v>
       </c>
     </row>
     <row r="123">
@@ -2517,16 +2517,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>11044.92520718014</v>
+        <v>11044.92520718023</v>
       </c>
       <c r="C123" t="n">
-        <v>106.0747038660777</v>
+        <v>106.0747038660323</v>
       </c>
       <c r="D123" t="n">
-        <v>8.886491434382716e-05</v>
+        <v>8.886489197011831e-05</v>
       </c>
       <c r="E123" t="n">
-        <v>46.17063292608698</v>
+        <v>46.17063292839116</v>
       </c>
     </row>
     <row r="124">
@@ -2534,16 +2534,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>10824.57305237325</v>
+        <v>10824.57305237258</v>
       </c>
       <c r="C124" t="n">
-        <v>29.4289920711501</v>
+        <v>29.42899207114792</v>
       </c>
       <c r="D124" t="n">
         <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>46.14863898632541</v>
+        <v>46.14863898715834</v>
       </c>
     </row>
     <row r="125">
@@ -2551,16 +2551,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>10727.99996126401</v>
+        <v>10727.99996126419</v>
       </c>
       <c r="C125" t="n">
-        <v>1.288029547321061e-05</v>
+        <v>1.288001384528335e-05</v>
       </c>
       <c r="D125" t="n">
-        <v>2.582985672610731e-05</v>
+        <v>2.582995007128308e-05</v>
       </c>
       <c r="E125" t="n">
-        <v>44.501806997982</v>
+        <v>44.50180699622415</v>
       </c>
     </row>
     <row r="126">
@@ -2568,7 +2568,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>10805.00153939816</v>
+        <v>10805.00153939799</v>
       </c>
       <c r="C126" t="n">
         <v>0</v>
@@ -2577,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>45.67354832665315</v>
+        <v>45.67354832293002</v>
       </c>
     </row>
     <row r="127">
@@ -2585,16 +2585,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>11149.99978827621</v>
+        <v>11149.99978827575</v>
       </c>
       <c r="C127" t="n">
-        <v>7.053944726065462e-05</v>
+        <v>7.054013588462091e-05</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0001410432904888927</v>
+        <v>0.0001410430815520733</v>
       </c>
       <c r="E127" t="n">
-        <v>47.85948040909165</v>
+        <v>47.85948041398147</v>
       </c>
     </row>
     <row r="128">
@@ -2602,16 +2602,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>11858.9981611997</v>
+        <v>11858.99816119978</v>
       </c>
       <c r="C128" t="n">
-        <v>0.0006120985760573726</v>
+        <v>0.0006120981054105023</v>
       </c>
       <c r="D128" t="n">
-        <v>0.001225476347304614</v>
+        <v>0.001225476747354214</v>
       </c>
       <c r="E128" t="n">
-        <v>63.43334517906574</v>
+        <v>63.43334517510583</v>
       </c>
     </row>
     <row r="129">
@@ -2619,7 +2619,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>13069.36803665496</v>
+        <v>13069.36803665217</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
@@ -2628,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="E129" t="n">
-        <v>1137.010122611129</v>
+        <v>1137.010122278067</v>
       </c>
     </row>
     <row r="130">
@@ -2636,7 +2636,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>14238.00276999098</v>
+        <v>14238.00276999149</v>
       </c>
       <c r="C130" t="n">
         <v>0</v>
@@ -2645,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="E130" t="n">
-        <v>71.22247053175711</v>
+        <v>71.2224705337628</v>
       </c>
     </row>
     <row r="131">
@@ -2653,7 +2653,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>15002.00561850373</v>
+        <v>15002.00561850352</v>
       </c>
       <c r="C131" t="n">
         <v>0</v>
@@ -2662,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="E131" t="n">
-        <v>101.4360923068469</v>
+        <v>101.4360923063467</v>
       </c>
     </row>
     <row r="132">
@@ -2670,7 +2670,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>15236.01810246381</v>
+        <v>15236.01810246252</v>
       </c>
       <c r="C132" t="n">
         <v>0</v>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="E132" t="n">
-        <v>101.935054908026</v>
+        <v>101.9350549083895</v>
       </c>
     </row>
     <row r="133">
@@ -2687,16 +2687,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>15212.99687662468</v>
+        <v>15212.996876624</v>
       </c>
       <c r="C133" t="n">
-        <v>0.001034560967629491</v>
+        <v>0.001034561976033661</v>
       </c>
       <c r="D133" t="n">
-        <v>0.002086727695634502</v>
+        <v>0.002086727381797455</v>
       </c>
       <c r="E133" t="n">
-        <v>101.8049920238848</v>
+        <v>101.8049920263608</v>
       </c>
     </row>
     <row r="134">
@@ -2704,7 +2704,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>14950.00175628483</v>
+        <v>14950.0017562844</v>
       </c>
       <c r="C134" t="n">
         <v>0</v>
@@ -2713,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="E134" t="n">
-        <v>74.59914177051961</v>
+        <v>74.59914176673219</v>
       </c>
     </row>
     <row r="135">
@@ -2721,16 +2721,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>14625.99994066686</v>
+        <v>14625.99994066676</v>
       </c>
       <c r="C135" t="n">
-        <v>1.976726253229532e-05</v>
+        <v>1.976742472906559e-05</v>
       </c>
       <c r="D135" t="n">
-        <v>3.952637466782544e-05</v>
+        <v>3.952629067077766e-05</v>
       </c>
       <c r="E135" t="n">
-        <v>72.4321376182136</v>
+        <v>72.43213761894316</v>
       </c>
     </row>
     <row r="136">
@@ -2738,7 +2738,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>14351.00007758948</v>
+        <v>14351.00007758976</v>
       </c>
       <c r="C136" t="n">
         <v>0</v>
@@ -2747,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="E136" t="n">
-        <v>71.17552552364116</v>
+        <v>71.17552552500783</v>
       </c>
     </row>
     <row r="137">
@@ -2755,16 +2755,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>14233.99998668078</v>
+        <v>14233.99998668096</v>
       </c>
       <c r="C137" t="n">
-        <v>4.458971571261561e-06</v>
+        <v>4.458520721331704e-06</v>
       </c>
       <c r="D137" t="n">
-        <v>8.85139545044097e-06</v>
+        <v>8.851665540347507e-06</v>
       </c>
       <c r="E137" t="n">
-        <v>70.82909872396341</v>
+        <v>70.82909872231983</v>
       </c>
     </row>
     <row r="138">
@@ -2772,16 +2772,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>14456.55854259462</v>
+        <v>14456.55854259427</v>
       </c>
       <c r="C138" t="n">
-        <v>25.44147437312193</v>
+        <v>25.44147437311626</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
       </c>
       <c r="E138" t="n">
-        <v>71.47602959978727</v>
+        <v>71.47602959622827</v>
       </c>
     </row>
     <row r="139">
@@ -2789,16 +2789,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>14895.29211426546</v>
+        <v>14895.29211426498</v>
       </c>
       <c r="C139" t="n">
-        <v>88.70819151970815</v>
+        <v>88.70819151975368</v>
       </c>
       <c r="D139" t="n">
         <v>0</v>
       </c>
       <c r="E139" t="n">
-        <v>74.1216375475431</v>
+        <v>74.12163754572791</v>
       </c>
     </row>
     <row r="140">
@@ -2806,16 +2806,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>15406.33843732344</v>
+        <v>15406.33843732363</v>
       </c>
       <c r="C140" t="n">
-        <v>224.6610055205092</v>
+        <v>224.661005520388</v>
       </c>
       <c r="D140" t="n">
-        <v>0.0005565994567490445</v>
+        <v>0.0005565993857492442</v>
       </c>
       <c r="E140" t="n">
-        <v>102.3595857288783</v>
+        <v>102.3595857299626</v>
       </c>
     </row>
     <row r="141">
@@ -2823,16 +2823,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>15196.55027172181</v>
+        <v>15196.55027172197</v>
       </c>
       <c r="C141" t="n">
-        <v>297.4574733228394</v>
+        <v>297.4574733228318</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>101.8157269480403</v>
+        <v>101.8157269464378</v>
       </c>
     </row>
     <row r="142">
@@ -2840,16 +2840,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>14687.65366940025</v>
+        <v>14687.65366939983</v>
       </c>
       <c r="C142" t="n">
-        <v>281.3462615655778</v>
+        <v>281.3462615658167</v>
       </c>
       <c r="D142" t="n">
-        <v>6.896519493802506e-05</v>
+        <v>6.896537048382508e-05</v>
       </c>
       <c r="E142" t="n">
-        <v>71.98524855656839</v>
+        <v>71.98524855400153</v>
       </c>
     </row>
     <row r="143">
@@ -2857,16 +2857,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>13905.42826535511</v>
+        <v>13905.42826535497</v>
       </c>
       <c r="C143" t="n">
-        <v>292.5712516569753</v>
+        <v>292.5712516569736</v>
       </c>
       <c r="D143" t="n">
-        <v>0.0004825054258894879</v>
+        <v>0.0004825055527615408</v>
       </c>
       <c r="E143" t="n">
-        <v>71.65526422582798</v>
+        <v>71.65526422463756</v>
       </c>
     </row>
     <row r="144">
@@ -2874,16 +2874,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>12915.40181934974</v>
+        <v>12915.40181934982</v>
       </c>
       <c r="C144" t="n">
-        <v>263.6099963424944</v>
+        <v>263.6099963424584</v>
       </c>
       <c r="D144" t="n">
         <v>0</v>
       </c>
       <c r="E144" t="n">
-        <v>70.84603786093072</v>
+        <v>70.84603786465192</v>
       </c>
     </row>
     <row r="145">
@@ -2891,16 +2891,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>11868.14016806736</v>
+        <v>11868.14016806751</v>
       </c>
       <c r="C145" t="n">
-        <v>250.8602205453771</v>
+        <v>250.8602205453954</v>
       </c>
       <c r="D145" t="n">
         <v>0</v>
       </c>
       <c r="E145" t="n">
-        <v>63.53122783424752</v>
+        <v>63.53122783377239</v>
       </c>
     </row>
     <row r="146">
@@ -2908,16 +2908,16 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>11016.16070514216</v>
+        <v>11016.16070514197</v>
       </c>
       <c r="C146" t="n">
-        <v>182.6214949417611</v>
+        <v>182.6214949417688</v>
       </c>
       <c r="D146" t="n">
         <v>0</v>
       </c>
       <c r="E146" t="n">
-        <v>1300.176297207794</v>
+        <v>1300.176224742928</v>
       </c>
     </row>
     <row r="147">
@@ -2925,16 +2925,16 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>9907.0121733299</v>
+        <v>9907.012173329949</v>
       </c>
       <c r="C147" t="n">
-        <v>195.9878263393168</v>
+        <v>195.9878263392946</v>
       </c>
       <c r="D147" t="n">
-        <v>3.304483191630012e-07</v>
+        <v>3.304186355859197e-07</v>
       </c>
       <c r="E147" t="n">
-        <v>41.59696818868396</v>
+        <v>41.59696819328044</v>
       </c>
     </row>
     <row r="148">
@@ -2942,16 +2942,16 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>10384.67653671446</v>
+        <v>10384.67653671427</v>
       </c>
       <c r="C148" t="n">
-        <v>226.3234996180008</v>
+        <v>226.3234996180105</v>
       </c>
       <c r="D148" t="n">
         <v>0</v>
       </c>
       <c r="E148" t="n">
-        <v>44.51415568236692</v>
+        <v>44.51415568319802</v>
       </c>
     </row>
     <row r="149">
@@ -2959,16 +2959,16 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>10054.62742307407</v>
+        <v>10054.62742307403</v>
       </c>
       <c r="C149" t="n">
-        <v>271.3725754676191</v>
+        <v>271.3725754676167</v>
       </c>
       <c r="D149" t="n">
-        <v>1.456863540826708e-06</v>
+        <v>1.456885237969402e-06</v>
       </c>
       <c r="E149" t="n">
-        <v>44.39642217200569</v>
+        <v>44.39642218200022</v>
       </c>
     </row>
     <row r="150">
@@ -2976,16 +2976,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>10106.96734813155</v>
+        <v>10106.96734813148</v>
       </c>
       <c r="C150" t="n">
-        <v>155.0326479464134</v>
+        <v>155.0326479464353</v>
       </c>
       <c r="D150" t="n">
-        <v>3.918134009248148e-06</v>
+        <v>3.918171407208163e-06</v>
       </c>
       <c r="E150" t="n">
-        <v>44.43690029414294</v>
+        <v>44.43690029392678</v>
       </c>
     </row>
     <row r="151">
@@ -2993,16 +2993,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>10048.68690284621</v>
+        <v>10048.68690284626</v>
       </c>
       <c r="C151" t="n">
-        <v>332.31318247605</v>
+        <v>332.3131824760396</v>
       </c>
       <c r="D151" t="n">
         <v>0</v>
       </c>
       <c r="E151" t="n">
-        <v>44.33306896394729</v>
+        <v>44.33306895737736</v>
       </c>
     </row>
     <row r="152">
@@ -3010,16 +3010,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>10277.81951687519</v>
+        <v>10277.81951687521</v>
       </c>
       <c r="C152" t="n">
-        <v>399.1804765839702</v>
+        <v>399.1804765839659</v>
       </c>
       <c r="D152" t="n">
-        <v>6.534297056650669e-06</v>
+        <v>6.534280864407036e-06</v>
       </c>
       <c r="E152" t="n">
-        <v>44.48747035259839</v>
+        <v>44.48747035342107</v>
       </c>
     </row>
     <row r="153">
@@ -3027,16 +3027,16 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>10754.19593795345</v>
+        <v>10754.19593795346</v>
       </c>
       <c r="C153" t="n">
-        <v>419.8040610272261</v>
+        <v>419.8040610272317</v>
       </c>
       <c r="D153" t="n">
-        <v>1.018326590524271e-06</v>
+        <v>1.01830760777381e-06</v>
       </c>
       <c r="E153" t="n">
-        <v>45.42573486976221</v>
+        <v>45.42573487017166</v>
       </c>
     </row>
     <row r="154">
@@ -3044,16 +3044,16 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>11716.42279370416</v>
+        <v>11716.42279370418</v>
       </c>
       <c r="C154" t="n">
-        <v>342.5772001642189</v>
+        <v>342.5772001642134</v>
       </c>
       <c r="D154" t="n">
-        <v>6.125474153729243e-06</v>
+        <v>6.125485758774838e-06</v>
       </c>
       <c r="E154" t="n">
-        <v>63.3524785780618</v>
+        <v>63.35247857772787</v>
       </c>
     </row>
     <row r="155">
@@ -3061,16 +3061,16 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>12728.33584951111</v>
+        <v>12728.33584951124</v>
       </c>
       <c r="C155" t="n">
-        <v>226.6639912165647</v>
+        <v>226.6639912165055</v>
       </c>
       <c r="D155" t="n">
-        <v>0.0001591131922854103</v>
+        <v>0.0001591131571700046</v>
       </c>
       <c r="E155" t="n">
-        <v>69.39933925497752</v>
+        <v>69.39933926275442</v>
       </c>
     </row>
     <row r="156">
@@ -3078,16 +3078,16 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>13442.41753177108</v>
+        <v>13442.41753177145</v>
       </c>
       <c r="C156" t="n">
-        <v>151.594890788877</v>
+        <v>151.5948907888582</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
       </c>
       <c r="E156" t="n">
-        <v>1930.767364005923</v>
+        <v>1930.767363717849</v>
       </c>
     </row>
     <row r="157">
@@ -3095,16 +3095,16 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>13895.21384324276</v>
+        <v>13895.21384324234</v>
       </c>
       <c r="C157" t="n">
-        <v>66.78670590467709</v>
+        <v>66.78670590471972</v>
       </c>
       <c r="D157" t="n">
         <v>0</v>
       </c>
       <c r="E157" t="n">
-        <v>70.69557803523652</v>
+        <v>70.69557804193097</v>
       </c>
     </row>
     <row r="158">
@@ -3112,16 +3112,16 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>14100.99989154207</v>
+        <v>14100.99989154216</v>
       </c>
       <c r="C158" t="n">
-        <v>3.617040667186398e-05</v>
+        <v>3.617034266768977e-05</v>
       </c>
       <c r="D158" t="n">
-        <v>7.221532423601342e-05</v>
+        <v>7.22152684985129e-05</v>
       </c>
       <c r="E158" t="n">
-        <v>70.87326084235805</v>
+        <v>70.87326085266389</v>
       </c>
     </row>
     <row r="159">
@@ -3129,7 +3129,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>14044.00066679572</v>
+        <v>14044.00066679259</v>
       </c>
       <c r="C159" t="n">
         <v>0</v>
@@ -3138,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="E159" t="n">
-        <v>70.83923196289474</v>
+        <v>70.83923195484734</v>
       </c>
     </row>
     <row r="160">
@@ -3146,7 +3146,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>13897.00005597542</v>
+        <v>13897.00005597845</v>
       </c>
       <c r="C160" t="n">
         <v>0</v>
@@ -3155,7 +3155,7 @@
         <v>0</v>
       </c>
       <c r="E160" t="n">
-        <v>70.70341952941246</v>
+        <v>70.70341952776644</v>
       </c>
     </row>
     <row r="161">
@@ -3163,16 +3163,16 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>13817.99989913966</v>
+        <v>13817.99989913954</v>
       </c>
       <c r="C161" t="n">
-        <v>3.363745511972355e-05</v>
+        <v>3.363737718530361e-05</v>
       </c>
       <c r="D161" t="n">
-        <v>6.715573531916864e-05</v>
+        <v>6.71559544749621e-05</v>
       </c>
       <c r="E161" t="n">
-        <v>70.50902446068939</v>
+        <v>70.50902446017156</v>
       </c>
     </row>
     <row r="162">
@@ -3180,7 +3180,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>14044.00121608796</v>
+        <v>14044.00121608746</v>
       </c>
       <c r="C162" t="n">
         <v>0</v>
@@ -3189,7 +3189,7 @@
         <v>0</v>
       </c>
       <c r="E162" t="n">
-        <v>70.70643922425113</v>
+        <v>70.70643922430799</v>
       </c>
     </row>
     <row r="163">
@@ -3197,16 +3197,16 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>14534.99989759713</v>
+        <v>14534.999897597</v>
       </c>
       <c r="C163" t="n">
-        <v>3.492431401330483e-05</v>
+        <v>3.492449219223237e-05</v>
       </c>
       <c r="D163" t="n">
-        <v>6.741116504106702e-05</v>
+        <v>6.741109295387639e-05</v>
       </c>
       <c r="E163" t="n">
-        <v>93.54623401984738</v>
+        <v>93.54623401913356</v>
       </c>
     </row>
     <row r="164">
@@ -3214,16 +3214,16 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>14996.99998962721</v>
+        <v>14996.99998962697</v>
       </c>
       <c r="C164" t="n">
-        <v>3.454651775279173e-06</v>
+        <v>3.454852858780114e-06</v>
       </c>
       <c r="D164" t="n">
-        <v>6.911202337765539e-06</v>
+        <v>6.911245611869398e-06</v>
       </c>
       <c r="E164" t="n">
-        <v>82.58594320731105</v>
+        <v>82.58594321501121</v>
       </c>
     </row>
     <row r="165">
@@ -3231,16 +3231,16 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>15633.99973902888</v>
+        <v>15633.99973902884</v>
       </c>
       <c r="C165" t="n">
-        <v>8.695076737794694e-05</v>
+        <v>8.695089097845142e-05</v>
       </c>
       <c r="D165" t="n">
-        <v>0.0001738464924855179</v>
+        <v>0.0001738464324041364</v>
       </c>
       <c r="E165" t="n">
-        <v>103.4190118934497</v>
+        <v>103.4190118868697</v>
       </c>
     </row>
     <row r="166">
@@ -3248,7 +3248,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>15558.0016453578</v>
+        <v>15558.00164535803</v>
       </c>
       <c r="C166" t="n">
         <v>0</v>
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="E166" t="n">
-        <v>103.2239682503589</v>
+        <v>103.2239682641738</v>
       </c>
     </row>
     <row r="167">
@@ -3265,7 +3265,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>14650.00018052818</v>
+        <v>14650.00018052811</v>
       </c>
       <c r="C167" t="n">
         <v>0</v>
@@ -3274,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="E167" t="n">
-        <v>73.05244894280467</v>
+        <v>73.0524489356352</v>
       </c>
     </row>
     <row r="168">
@@ -3282,7 +3282,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>13470.00010446429</v>
+        <v>13470.00010446427</v>
       </c>
       <c r="C168" t="n">
         <v>0</v>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="E168" t="n">
-        <v>70.53772814337371</v>
+        <v>70.53772814495412</v>
       </c>
     </row>
     <row r="169">
@@ -3299,7 +3299,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>12278.00000063408</v>
+        <v>12278.00000063393</v>
       </c>
       <c r="C169" t="n">
         <v>0</v>
@@ -3308,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="E169" t="n">
-        <v>101.2517099698829</v>
+        <v>101.2517099705902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>